<commit_message>
Count and Masks support
</commit_message>
<xml_diff>
--- a/examples/example.xlsx
+++ b/examples/example.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Example" sheetId="1" r:id="rId3"/>
+    <sheet state="visible" name="Example2" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Title</t>
   </si>
@@ -19,10 +20,31 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Example Title</t>
-  </si>
-  <si>
-    <t>Example Description</t>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Card 3</t>
+  </si>
+  <si>
+    <t>Example Description 3</t>
+  </si>
+  <si>
+    <t>Card 4</t>
+  </si>
+  <si>
+    <t>Example Description 4</t>
+  </si>
+  <si>
+    <t>Card 1</t>
+  </si>
+  <si>
+    <t>Example Description 1</t>
+  </si>
+  <si>
+    <t>Card 2</t>
+  </si>
+  <si>
+    <t>Example Description 2</t>
   </si>
 </sst>
 </file>
@@ -56,12 +78,15 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -75,8 +100,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -92,13 +124,81 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="25.14"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>